<commit_message>
started working on GLS for gene expression
</commit_message>
<xml_diff>
--- a/data/tests/cluster_13.xlsx
+++ b/data/tests/cluster_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -667,6 +667,63 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Rv0554</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>bpoC Rv0554</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Rv2940c</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>mas Rv2940c</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Rv2808</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Rv2808</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>